<commit_message>
Running first tests using excel data
</commit_message>
<xml_diff>
--- a/testautomation/src/main/resources/SourceDataFiles/HotelResData.xlsx
+++ b/testautomation/src/main/resources/SourceDataFiles/HotelResData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t xml:space="preserve">IdHotelRes</t>
   </si>
@@ -64,10 +64,13 @@
     <t xml:space="preserve">Cancun</t>
   </si>
   <si>
-    <t xml:space="preserve">20/02/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22/02/2019</t>
+    <t xml:space="preserve">10/02/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/02/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">HR002</t>
@@ -89,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">HR005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">HR006</t>
@@ -205,8 +211,8 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1:O17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -267,8 +273,8 @@
       <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>1</v>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>0</v>
@@ -294,19 +300,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>0</v>
@@ -332,10 +338,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -343,8 +349,8 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>1</v>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>0</v>
@@ -370,10 +376,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -381,8 +387,8 @@
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>1</v>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>0</v>
@@ -408,7 +414,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -419,14 +425,14 @@
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>2</v>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>0</v>
@@ -446,10 +452,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -457,14 +463,14 @@
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>2</v>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>0</v>
@@ -484,25 +490,25 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="F8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>0</v>
@@ -522,10 +528,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -533,14 +539,14 @@
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>2</v>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed tabs error, Add support to test.pt.com.mx
</commit_message>
<xml_diff>
--- a/testautomation/src/main/resources/SourceDataFiles/HotelResData.xlsx
+++ b/testautomation/src/main/resources/SourceDataFiles/HotelResData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t xml:space="preserve">IdHotelRes</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">HR001</t>
   </si>
   <si>
-    <t xml:space="preserve">Cancun</t>
+    <t xml:space="preserve">Cancún (y alrededores), México</t>
   </si>
   <si>
     <t xml:space="preserve">10/02/2019</t>
@@ -76,25 +76,22 @@
     <t xml:space="preserve">HR002</t>
   </si>
   <si>
-    <t xml:space="preserve">Ciudad de Mexico</t>
+    <t xml:space="preserve">Ciudad de México (y alrededores), Distrito Federal, México</t>
   </si>
   <si>
     <t xml:space="preserve">HR003</t>
   </si>
   <si>
-    <t xml:space="preserve">Bogota</t>
+    <t xml:space="preserve">Bogotá (y alrededores), Colombia</t>
   </si>
   <si>
     <t xml:space="preserve">HR004</t>
   </si>
   <si>
-    <t xml:space="preserve">Los Angeles</t>
+    <t xml:space="preserve">Los Ángeles (y alrededores), California, Estados Unidos de América</t>
   </si>
   <si>
     <t xml:space="preserve">HR005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">HR006</t>
@@ -218,7 +215,7 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="56.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -426,7 +423,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>0</v>
@@ -452,7 +449,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
@@ -464,7 +461,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>0</v>
@@ -490,7 +487,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -502,7 +499,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>0</v>
@@ -528,7 +525,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
@@ -540,7 +537,7 @@
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Creating functions for componenet SPAHLWidget. Refactor of name of tests and workflows.
</commit_message>
<xml_diff>
--- a/testautomation/src/main/resources/SourceDataFiles/HotelResData.xlsx
+++ b/testautomation/src/main/resources/SourceDataFiles/HotelResData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t xml:space="preserve">IdHotelRes</t>
   </si>
@@ -64,34 +64,40 @@
     <t xml:space="preserve">Cancún (y alrededores), México</t>
   </si>
   <si>
+    <t xml:space="preserve">04/02/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/02/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciudad de México (y alrededores), Distrito Federal, México</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bogotá (y alrededores), Colombia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los Ángeles (y alrededores), California, Estados Unidos de América</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR005</t>
+  </si>
+  <si>
     <t xml:space="preserve">10/02/2019</t>
   </si>
   <si>
     <t xml:space="preserve">12/02/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ciudad de México (y alrededores), Distrito Federal, México</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bogotá (y alrededores), Colombia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los Ángeles (y alrededores), California, Estados Unidos de América</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR005</t>
   </si>
   <si>
     <t xml:space="preserve">HR006</t>
@@ -208,14 +214,14 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="56.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="56.16"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -417,10 +423,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -449,16 +455,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -487,16 +493,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
@@ -525,16 +531,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>

</xml_diff>